<commit_message>
More RAS Survey Automation
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/RASScenario4.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/RASScenario4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bucurgb/IdeaProjects/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9DFAA6-7CFF-0440-B9CE-E40F0F3286DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03316FD-8AA5-0D42-9CFC-B167B390F02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27540" yWindow="500" windowWidth="40760" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27080" yWindow="500" windowWidth="40760" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="screenerScenario4" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="1953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2362" uniqueCount="2133">
   <si>
     <t>Question</t>
   </si>
@@ -4878,53 +4878,15 @@
     <t>Do you have any issues with curving of the spine?  This would often be diagnosed or evaluated by an orthopaedic surgeon.  Examples include scoliosis and kyphosis.</t>
   </si>
   <si>
-    <t>Have you ever been diagnosed with any of the following types of curvature of the spine? 
-Please select all that apply. Option 1</t>
-  </si>
-  <si>
     <t>Scoliosis (curving of the spine from side to side)</t>
   </si>
   <si>
-    <t>Have you ever been diagnosed with any of the following types of curvature of the spine? 
-Please select all that apply. Option 2</t>
-  </si>
-  <si>
     <t>Kyphosis (curving of the spine from front to back)</t>
   </si>
   <si>
-    <t>Have you ever been diagnosed with any of the following types of curvature of the spine? 
-Please select all that apply. Option 3</t>
-  </si>
-  <si>
     <t>Kyphoscoliosis (curving of the spine both side to side and front to back)</t>
   </si>
   <si>
-    <t>Have you ever been diagnosed with any of the following types of curvature of the spine? 
-Please select all that apply. Option 4</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both).  If you do not recall the details, place an 'X' in the column 'Don't know'.  For the treatment column, if no treatment was required, please write 'None'. Other Column 1</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both).  If you do not recall the details, place an 'X' in the column 'Don't know'.  For the treatment column, if no treatment was required, please write 'None'. Other Column 2</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both).  If you do not recall the details, place an 'X' in the column 'Don't know'.  For the treatment column, if no treatment was required, please write 'None'. Other Column 3</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both).  If you do not recall the details, place an 'X' in the column 'Don't know'.  For the treatment column, if no treatment was required, please write 'None'. Other Column 4</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both).  If you do not recall the details, place an 'X' in the column 'Don't know'.  For the treatment column, if no treatment was required, please write 'None'. Other Column 5</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both).  If you do not recall the details, place an 'X' in the column 'Don't know'.  For the treatment column, if no treatment was required, please write 'None'. Other Column 6</t>
-  </si>
-  <si>
-    <t>Has your neck been described as short or webbed?
-Individuals with a short, webbed neck may have a low hairline or extra skin where the neck meets the shoulders.</t>
-  </si>
-  <si>
     <t>Have you ever been diagnosed with joint issues?  These conditions are often diagnosed by neurologists, rheumatologists and orthopaedic surgeons.  Examples include ulnar deviation, Achilles tendon contracture, hip dysplasia.</t>
   </si>
   <si>
@@ -4961,75 +4923,9 @@
     <t>Have you ever been diagnosed with the following joint issues?  Please select all that apply. Option 6</t>
   </si>
   <si>
-    <t>Please complete the table below for each of the joint issues listed.  For each condition, please include the date or age when symptoms first occurred and date or age at diagnosis (you do not need to include both the date and age).  If you do not recall the details, please place an 'X' in the column 'Don't know.'  If no treatment was required, please put 'None' in the 'Treatment' column. Other Column 1</t>
-  </si>
-  <si>
-    <t>cdvdfb</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the joint issues listed.  For each condition, please include the date or age when symptoms first occurred and date or age at diagnosis (you do not need to include both the date and age).  If you do not recall the details, please place an 'X' in the column 'Don't know.'  If no treatment was required, please put 'None' in the 'Treatment' column. Other Column 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fg bfh g </t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the joint issues listed.  For each condition, please include the date or age when symptoms first occurred and date or age at diagnosis (you do not need to include both the date and age).  If you do not recall the details, please place an 'X' in the column 'Don't know.'  If no treatment was required, please put 'None' in the 'Treatment' column. Other Column 3</t>
-  </si>
-  <si>
-    <t>hnmn nymy</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the joint issues listed.  For each condition, please include the date or age when symptoms first occurred and date or age at diagnosis (you do not need to include both the date and age).  If you do not recall the details, please place an 'X' in the column 'Don't know.'  If no treatment was required, please put 'None' in the 'Treatment' column. Other Column 4</t>
-  </si>
-  <si>
-    <t>yukm66jk</t>
-  </si>
-  <si>
-    <t>lease complete the table below for each of the joint issues listed.  For each condition, please include the date or age when symptoms first occurred and date or age at diagnosis (you do not need to include both the date and age).  If you do not recall the details, please place an 'X' in the column 'Don't know.'  If no treatment was required, please put 'None' in the 'Treatment' column. Other Column 5</t>
-  </si>
-  <si>
-    <t>7j67ijntn</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the joint issues listed.  For each condition, please include the date or age when symptoms first occurred and date or age at diagnosis (you do not need to include both the date and age).  If you do not recall the details, please place an 'X' in the column 'Don't know.'  If no treatment was required, please put 'None' in the 'Treatment' column. Other Column 6</t>
-  </si>
-  <si>
-    <t>uyjumy</t>
-  </si>
-  <si>
-    <t>lease complete the table below for each of the joint issues listed.  For each condition, please include the date or age when symptoms first occurred and date or age at diagnosis (you do not need to include both the date and age).  If you do not recall the details, please place an 'X' in the column 'Don't know.'  If no treatment was required, please put 'None' in the 'Treatment' column. Other Column 7</t>
-  </si>
-  <si>
-    <t>7ujmy7ui79</t>
-  </si>
-  <si>
     <t>The next set of questions ask about blood disorders.  Blood disorders include immune system problems (white blood cells) or bleeding/clotting issues (platelets) or other bone marrow problems (where white blood cells, red blood cells and platelets are produced).</t>
   </si>
   <si>
-    <t>Have you ever had an evaluation by a hematologist or oncologist?  Hematologists are physicians who specialize in the blood system, including white blood cells, platelets, red blood cells and clotting factors.  Oncologists are physicians who specialize in cancer.</t>
-  </si>
-  <si>
-    <t>Please provide the information below for the hematologist/oncologist who completed your evaluation. Name</t>
-  </si>
-  <si>
-    <t>fnhumy7</t>
-  </si>
-  <si>
-    <t>Please provide the information below for the hematologist/oncologist who completed your evaluation. Location</t>
-  </si>
-  <si>
-    <t>9p/.iu.</t>
-  </si>
-  <si>
-    <t>Please provide the information below for the hematologist/oncologist who completed your evaluation. Hospital</t>
-  </si>
-  <si>
-    <t>o/kkk;/k</t>
-  </si>
-  <si>
-    <t>Do you have issues with bleeding or bruising?  Examples include easy bruising, poor blood clotting.  These conditions are often evaluated and diagnosed by a hematologist (a physician who specializes in the blood).</t>
-  </si>
-  <si>
     <t>Do you have any of the following issues with bleeding or bruising?  Please select all that apply. Option 1</t>
   </si>
   <si>
@@ -5040,57 +4936,6 @@
   </si>
   <si>
     <t>Do you have any of the following issues with bleeding or bruising?  Please select all that apply. Option 4</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the bleeding/bruising issues listed.  For each condition, please provide your age or date when symptoms first started and at diagnosis (you only need to provide date or age, but not both).  If you do not recall the details, please place an 'X' in the 'Don't know' column.  If no treatment was required, please write 'None' in the treatment column.  other Column 1</t>
-  </si>
-  <si>
-    <t>ghnyurmfy</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the bleeding/bruising issues listed.  For each condition, please provide your age or date when symptoms first started and at diagnosis (you only need to provide date or age, but not both).  If you do not recall the details, please place an 'X' in the 'Don't know' column.  If no treatment was required, please write 'None' in the treatment column.  other Column 2</t>
-  </si>
-  <si>
-    <t>uktum</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the bleeding/bruising issues listed.  For each condition, please provide your age or date when symptoms first started and at diagnosis (you only need to provide date or age, but not both).  If you do not recall the details, please place an 'X' in the 'Don't know' column.  If no treatment was required, please write 'None' in the treatment column.  other Column 3</t>
-  </si>
-  <si>
-    <t>9p79l689</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the bleeding/bruising issues listed.  For each condition, please provide your age or date when symptoms first started and at diagnosis (you only need to provide date or age, but not both).  If you do not recall the details, please place an 'X' in the 'Don't know' column.  If no treatment was required, please write 'None' in the treatment column.  other Column 4</t>
-  </si>
-  <si>
-    <t>0009p89</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the bleeding/bruising issues listed.  For each condition, please provide your age or date when symptoms first started and at diagnosis (you only need to provide date or age, but not both).  If you do not recall the details, please place an 'X' in the 'Don't know' column.  If no treatment was required, please write 'None' in the treatment column.  other Column 5</t>
-  </si>
-  <si>
-    <t>uolu,i.o</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the bleeding/bruising issues listed.  For each condition, please provide your age or date when symptoms first started and at diagnosis (you only need to provide date or age, but not both).  If you do not recall the details, please place an 'X' in the 'Don't know' column.  If no treatment was required, please write 'None' in the treatment column.  other Column 6</t>
-  </si>
-  <si>
-    <t>jk,l.pop/</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the bleeding/bruising issues listed.  For each condition, please provide your age or date when symptoms first started and at diagnosis (you only need to provide date or age, but not both).  If you do not recall the details, please place an 'X' in the 'Don't know' column.  If no treatment was required, please write 'None' in the treatment column.  other Column 7</t>
-  </si>
-  <si>
-    <t>op/o/o/p</t>
-  </si>
-  <si>
-    <t>Please complete the table below for each of the bleeding/bruising issues listed.  For each condition, please provide your age or date when symptoms first started and at diagnosis (you only need to provide date or age, but not both).  If you do not recall the details, please place an 'X' in the 'Don't know' column.  If no treatment was required, please write 'None' in the treatment column.  other Column 8</t>
-  </si>
-  <si>
-    <t>hnngmyu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you have any known blood disorders or symptoms of blood disorders?  Examples include an enlarged spleen, leukemia, low platelets or low blood cells.  </t>
   </si>
   <si>
     <t>Have you ever been diagnosed with any of the following blood disorders or symptoms of blood disorders?  Please select all that apply. Option 1</t>
@@ -6069,10 +5914,700 @@
     <t>Test438</t>
   </si>
   <si>
-    <t>Test439</t>
-  </si>
-  <si>
-    <t>Test440</t>
+    <t>Have you been diagnosed with any of the following skeletal findings in the thoracic area? The thoracic area includes the chest and ribs. Please select all that apply. Option 4 Other</t>
+  </si>
+  <si>
+    <t>Test441</t>
+  </si>
+  <si>
+    <t>Test444</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with any of the following types of curvature of the spine? Please select all that apply. Option 4 Other</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with any of the following types of curvature of the spine? Please select all that apply. Option 4</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with any of the following types of curvature of the spine? Please select all that apply. Option 3</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with any of the following types of curvature of the spine? Please select all that apply. Option 2</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with any of the following types of curvature of the spine? Please select all that apply. Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 1 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 1 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 1 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 1 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 2 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 2 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 2 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 2 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 3 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 3 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 3 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 3 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 4 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 4 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 4 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 4 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 5 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 5 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 5 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 5 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 6 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 6 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 6 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 6 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 7 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 7 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 7 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the spine issues listed.  For each condition, please indicate your age or date when they occurred (you do not need to include both). Other Column 7 Option 4</t>
+  </si>
+  <si>
+    <t>Test447</t>
+  </si>
+  <si>
+    <t>Test448</t>
+  </si>
+  <si>
+    <t>Test449</t>
+  </si>
+  <si>
+    <t>Test450</t>
+  </si>
+  <si>
+    <t>Test451</t>
+  </si>
+  <si>
+    <t>Test452</t>
+  </si>
+  <si>
+    <t>Test453</t>
+  </si>
+  <si>
+    <t>Test454</t>
+  </si>
+  <si>
+    <t>Test455</t>
+  </si>
+  <si>
+    <t>Test456</t>
+  </si>
+  <si>
+    <t>Test457</t>
+  </si>
+  <si>
+    <t>Test458</t>
+  </si>
+  <si>
+    <t>Test459</t>
+  </si>
+  <si>
+    <t>Test460</t>
+  </si>
+  <si>
+    <t>Test461</t>
+  </si>
+  <si>
+    <t>Test462</t>
+  </si>
+  <si>
+    <t>Test463</t>
+  </si>
+  <si>
+    <t>Test464</t>
+  </si>
+  <si>
+    <t>Test465</t>
+  </si>
+  <si>
+    <t>Test466</t>
+  </si>
+  <si>
+    <t>Test467</t>
+  </si>
+  <si>
+    <t>Test468</t>
+  </si>
+  <si>
+    <t>Test469</t>
+  </si>
+  <si>
+    <t>Test470</t>
+  </si>
+  <si>
+    <t>Test471</t>
+  </si>
+  <si>
+    <t>Test472</t>
+  </si>
+  <si>
+    <t>Has your neck been described as short or webbed?</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with the following joint issues?  Please select all that apply. Option 6 Other</t>
+  </si>
+  <si>
+    <t>Test473</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 1 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 1 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 1 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 1 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 1 Option 5</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 1 Option 6</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 2 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 2 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 2 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 2 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 2 Option 5</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 2 Option 6</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 3 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 3 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 3 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 3 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 3 Option 5</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 3 Option 6</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 4 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 4 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 4 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 4 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 4 Option 5</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 4 Option 6</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 5 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 5 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 5 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 5 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 5 Option 5</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 5 Option 6</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 6 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 6 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 6 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 6 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 6 Option 5</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 6 Option 6</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 7 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 7 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 7 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 7 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 7 Option 5</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the joint issues listed. Column 7 Option 6</t>
+  </si>
+  <si>
+    <t>Test474</t>
+  </si>
+  <si>
+    <t>Test475</t>
+  </si>
+  <si>
+    <t>Test476</t>
+  </si>
+  <si>
+    <t>Test477</t>
+  </si>
+  <si>
+    <t>Test478</t>
+  </si>
+  <si>
+    <t>Test479</t>
+  </si>
+  <si>
+    <t>Test480</t>
+  </si>
+  <si>
+    <t>Test481</t>
+  </si>
+  <si>
+    <t>Test482</t>
+  </si>
+  <si>
+    <t>Test483</t>
+  </si>
+  <si>
+    <t>Test484</t>
+  </si>
+  <si>
+    <t>Test485</t>
+  </si>
+  <si>
+    <t>Test486</t>
+  </si>
+  <si>
+    <t>Test487</t>
+  </si>
+  <si>
+    <t>Test488</t>
+  </si>
+  <si>
+    <t>Test489</t>
+  </si>
+  <si>
+    <t>Test490</t>
+  </si>
+  <si>
+    <t>Test491</t>
+  </si>
+  <si>
+    <t>Test492</t>
+  </si>
+  <si>
+    <t>Test493</t>
+  </si>
+  <si>
+    <t>Test494</t>
+  </si>
+  <si>
+    <t>Test495</t>
+  </si>
+  <si>
+    <t>Test496</t>
+  </si>
+  <si>
+    <t>Test497</t>
+  </si>
+  <si>
+    <t>Test498</t>
+  </si>
+  <si>
+    <t>Test499</t>
+  </si>
+  <si>
+    <t>Test500</t>
+  </si>
+  <si>
+    <t>Test501</t>
+  </si>
+  <si>
+    <t>Test502</t>
+  </si>
+  <si>
+    <t>Test503</t>
+  </si>
+  <si>
+    <t>Test504</t>
+  </si>
+  <si>
+    <t>Test505</t>
+  </si>
+  <si>
+    <t>Test506</t>
+  </si>
+  <si>
+    <t>Test507</t>
+  </si>
+  <si>
+    <t>Test508</t>
+  </si>
+  <si>
+    <t>Test509</t>
+  </si>
+  <si>
+    <t>Test510</t>
+  </si>
+  <si>
+    <t>Test511</t>
+  </si>
+  <si>
+    <t>Test512</t>
+  </si>
+  <si>
+    <t>Test513</t>
+  </si>
+  <si>
+    <t>Test514</t>
+  </si>
+  <si>
+    <t>Test515</t>
+  </si>
+  <si>
+    <t>The next set of questions ask about blood disorders.</t>
+  </si>
+  <si>
+    <t>Have you ever had an evaluation by a hematologist or oncologist?</t>
+  </si>
+  <si>
+    <t>Please provide the information below for the hematologist oncologist who completed your evaluation. Name</t>
+  </si>
+  <si>
+    <t>Please provide the information below for the hematologist oncologist who completed your evaluation. Location</t>
+  </si>
+  <si>
+    <t>Please provide the information below for the hematologist oncologist who completed your evaluation. Hospital</t>
+  </si>
+  <si>
+    <t>Test516</t>
+  </si>
+  <si>
+    <t>Test517</t>
+  </si>
+  <si>
+    <t>Test518</t>
+  </si>
+  <si>
+    <t>Do you have issues with bleeding or bruising?</t>
+  </si>
+  <si>
+    <t>Easy bruising (bruising with little or no trauma)</t>
+  </si>
+  <si>
+    <t>Platelet dysfunction (an issue with your blood clotting too slowly due to problems with platelets (a type of blood cell) not working correctly. It may also cause easy bleeding</t>
+  </si>
+  <si>
+    <t>Clotting disorder (an issue with your blood clotting too slow due to problems with coagulation or clotting factors, may cause easy or excessive bleeding; includes factor VIII deficiency, factor XI deficiency, factor XII deficiency)</t>
+  </si>
+  <si>
+    <t>Do you have any of the following issues with bleeding or bruising?  Please select all that apply. Option 4 Other</t>
+  </si>
+  <si>
+    <t>Test519</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 1 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 1 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 1 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 1 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 2 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 2 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 2 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 2 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 3 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 3 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 3 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 3 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 4 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 4 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 4 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 4 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 5 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 5 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 5 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 5 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 6 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 6 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 6 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 6 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 7 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 7 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 7 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 7 Option 4</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 8 Option 1</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 8 Option 2</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 8 Option 3</t>
+  </si>
+  <si>
+    <t>Please complete the table below for each of the bleeding bruising issues listed Column 8 Option 4</t>
+  </si>
+  <si>
+    <t>Test520</t>
+  </si>
+  <si>
+    <t>Test521</t>
+  </si>
+  <si>
+    <t>Test522</t>
+  </si>
+  <si>
+    <t>Test523</t>
+  </si>
+  <si>
+    <t>Test524</t>
+  </si>
+  <si>
+    <t>Test525</t>
+  </si>
+  <si>
+    <t>Test526</t>
+  </si>
+  <si>
+    <t>Test527</t>
+  </si>
+  <si>
+    <t>Test528</t>
+  </si>
+  <si>
+    <t>Test529</t>
+  </si>
+  <si>
+    <t>Test530</t>
+  </si>
+  <si>
+    <t>Test531</t>
+  </si>
+  <si>
+    <t>Test532</t>
+  </si>
+  <si>
+    <t>Test533</t>
+  </si>
+  <si>
+    <t>Test534</t>
+  </si>
+  <si>
+    <t>Test535</t>
+  </si>
+  <si>
+    <t>Test536</t>
+  </si>
+  <si>
+    <t>Test537</t>
+  </si>
+  <si>
+    <t>Test538</t>
+  </si>
+  <si>
+    <t>Test539</t>
+  </si>
+  <si>
+    <t>Test540</t>
+  </si>
+  <si>
+    <t>Test541</t>
+  </si>
+  <si>
+    <t>Test542</t>
+  </si>
+  <si>
+    <t>Test544</t>
+  </si>
+  <si>
+    <t>Test543</t>
+  </si>
+  <si>
+    <t>Test545</t>
+  </si>
+  <si>
+    <t>Test546</t>
+  </si>
+  <si>
+    <t>Test547</t>
+  </si>
+  <si>
+    <t>Test548</t>
+  </si>
+  <si>
+    <t>Test549</t>
+  </si>
+  <si>
+    <t>Test550</t>
+  </si>
+  <si>
+    <t>Test551</t>
+  </si>
+  <si>
+    <t>Do you have any known blood disorders or symptoms of blood disorders?</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with any of the following blood disorders or symptoms of blood disorders?  Please select all that apply. Option 7 Other</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with any of the following blood disorders or symptoms of blood disorders?  Please select all that apply. Option 8 Other</t>
+  </si>
+  <si>
+    <t>Test552</t>
+  </si>
+  <si>
+    <t>Test553</t>
   </si>
 </sst>
 </file>
@@ -7488,15 +8023,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF90E83-6BB8-1941-861C-D1AD2F062745}">
-  <dimension ref="A1:B990"/>
+  <dimension ref="A1:B1078"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A755" workbookViewId="0">
-      <selection activeCell="B794" sqref="B794"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="A923" sqref="A923"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="98.1640625" customWidth="1"/>
+    <col min="1" max="1" width="162.83203125" customWidth="1"/>
     <col min="2" max="2" width="94" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8702,10 +9237,10 @@
     </row>
     <row r="151" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
-        <v>1929</v>
+        <v>1879</v>
       </c>
       <c r="B151" t="s">
-        <v>1930</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="68" x14ac:dyDescent="0.2">
@@ -9014,7 +9549,7 @@
         <v>507</v>
       </c>
       <c r="B190" t="s">
-        <v>1931</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -13489,7 +14024,7 @@
     </row>
     <row r="752" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A752" s="1" t="s">
-        <v>1932</v>
+        <v>1882</v>
       </c>
       <c r="B752" t="s">
         <v>12</v>
@@ -13500,7 +14035,7 @@
         <v>1524</v>
       </c>
       <c r="B753" t="s">
-        <v>1933</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="754" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -13508,7 +14043,7 @@
         <v>1525</v>
       </c>
       <c r="B754" t="s">
-        <v>1934</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="755" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -13516,7 +14051,7 @@
         <v>1526</v>
       </c>
       <c r="B755" t="s">
-        <v>1935</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="756" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -13577,10 +14112,10 @@
     </row>
     <row r="763" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A763" s="1" t="s">
-        <v>1936</v>
+        <v>1886</v>
       </c>
       <c r="B763" t="s">
-        <v>1937</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="764" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -13601,10 +14136,10 @@
     </row>
     <row r="766" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A766" s="1" t="s">
-        <v>1942</v>
+        <v>1892</v>
       </c>
       <c r="B766" t="s">
-        <v>1945</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="767" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -13617,15 +14152,15 @@
     </row>
     <row r="768" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A768" s="1" t="s">
-        <v>1943</v>
+        <v>1893</v>
       </c>
       <c r="B768" t="s">
-        <v>1944</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="769" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A769" s="1" t="s">
-        <v>1938</v>
+        <v>1888</v>
       </c>
       <c r="B769" t="s">
         <v>1543</v>
@@ -13673,15 +14208,15 @@
     </row>
     <row r="775" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A775" s="1" t="s">
-        <v>1940</v>
+        <v>1890</v>
       </c>
       <c r="B775" t="s">
-        <v>1941</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="776" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A776" s="3" t="s">
-        <v>1939</v>
+        <v>1889</v>
       </c>
       <c r="B776" s="12" t="s">
         <v>1553</v>
@@ -13689,7 +14224,7 @@
     </row>
     <row r="777" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A777" s="3" t="s">
-        <v>1946</v>
+        <v>1896</v>
       </c>
       <c r="B777" t="s">
         <v>12</v>
@@ -13700,7 +14235,7 @@
         <v>1554</v>
       </c>
       <c r="B778" t="s">
-        <v>1947</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="779" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -13708,7 +14243,7 @@
         <v>1555</v>
       </c>
       <c r="B779" t="s">
-        <v>1948</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="780" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -13716,7 +14251,7 @@
         <v>1556</v>
       </c>
       <c r="B780" t="s">
-        <v>1949</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="781" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -13753,1635 +14288,2346 @@
     </row>
     <row r="785" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A785" s="1" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B785" t="s">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="786" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A786" s="1" t="s">
         <v>1564</v>
       </c>
-      <c r="B785" t="s">
+      <c r="B786" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="786" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A786" s="3" t="s">
-        <v>1565</v>
-      </c>
-      <c r="B786" t="s">
-        <v>1566</v>
       </c>
     </row>
     <row r="787" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A787" s="3" t="s">
-        <v>1567</v>
+        <v>1908</v>
       </c>
       <c r="B787" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="788" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A788" s="3" t="s">
-        <v>1569</v>
+        <v>1907</v>
       </c>
       <c r="B788" t="s">
-        <v>1570</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="789" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A789" s="3" t="s">
-        <v>1571</v>
+        <v>1906</v>
       </c>
       <c r="B789" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="790" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A790" s="3" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B790" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="790" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A790" s="3" t="s">
-        <v>1572</v>
-      </c>
-      <c r="B790" t="s">
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="791" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+    <row r="791" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A791" s="3" t="s">
-        <v>1573</v>
+        <v>1904</v>
       </c>
       <c r="B791" t="s">
-        <v>1951</v>
-      </c>
-    </row>
-    <row r="792" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="792" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A792" s="3" t="s">
-        <v>1574</v>
+        <v>1909</v>
       </c>
       <c r="B792" t="s">
-        <v>1952</v>
-      </c>
-    </row>
-    <row r="793" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="793" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A793" s="3" t="s">
-        <v>1575</v>
+        <v>1910</v>
       </c>
       <c r="B793" t="s">
-        <v>1941</v>
-      </c>
-    </row>
-    <row r="794" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="794" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A794" s="3" t="s">
-        <v>1576</v>
+        <v>1911</v>
       </c>
       <c r="B794" t="s">
-        <v>1944</v>
-      </c>
-    </row>
-    <row r="795" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="795" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A795" s="3" t="s">
-        <v>1577</v>
+        <v>1912</v>
       </c>
       <c r="B795" t="s">
-        <v>1945</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="796" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A796" s="3" t="s">
-        <v>1578</v>
+        <v>1913</v>
       </c>
       <c r="B796" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="797" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="797" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A797" s="3" t="s">
-        <v>1579</v>
+        <v>1914</v>
       </c>
       <c r="B797" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="798" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="798" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A798" s="3" t="s">
-        <v>1580</v>
+        <v>1915</v>
       </c>
       <c r="B798" t="s">
-        <v>1581</v>
-      </c>
-    </row>
-    <row r="799" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="799" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A799" s="3" t="s">
-        <v>1582</v>
+        <v>1916</v>
       </c>
       <c r="B799" t="s">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="800" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1942</v>
+      </c>
+    </row>
+    <row r="800" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A800" s="3" t="s">
-        <v>1584</v>
+        <v>1917</v>
       </c>
       <c r="B800" t="s">
-        <v>1585</v>
-      </c>
-    </row>
-    <row r="801" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1943</v>
+      </c>
+    </row>
+    <row r="801" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A801" s="3" t="s">
-        <v>1586</v>
+        <v>1918</v>
       </c>
       <c r="B801" t="s">
-        <v>1587</v>
-      </c>
-    </row>
-    <row r="802" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="802" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A802" s="3" t="s">
-        <v>1588</v>
+        <v>1919</v>
       </c>
       <c r="B802" t="s">
-        <v>1589</v>
-      </c>
-    </row>
-    <row r="803" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="803" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A803" s="3" t="s">
-        <v>1590</v>
+        <v>1920</v>
       </c>
       <c r="B803" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="804" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="804" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A804" s="3" t="s">
-        <v>1591</v>
+        <v>1921</v>
       </c>
       <c r="B804" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="805" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1947</v>
+      </c>
+    </row>
+    <row r="805" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A805" s="3" t="s">
-        <v>1593</v>
+        <v>1922</v>
       </c>
       <c r="B805" t="s">
-        <v>1594</v>
-      </c>
-    </row>
-    <row r="806" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1948</v>
+      </c>
+    </row>
+    <row r="806" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A806" s="3" t="s">
-        <v>1595</v>
+        <v>1923</v>
       </c>
       <c r="B806" t="s">
-        <v>1596</v>
-      </c>
-    </row>
-    <row r="807" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="807" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A807" s="3" t="s">
-        <v>1597</v>
+        <v>1924</v>
       </c>
       <c r="B807" t="s">
-        <v>1598</v>
-      </c>
-    </row>
-    <row r="808" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A808" s="1" t="s">
-        <v>1599</v>
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="808" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A808" s="3" t="s">
+        <v>1925</v>
       </c>
       <c r="B808" t="s">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="809" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="809" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A809" s="3" t="s">
-        <v>1601</v>
+        <v>1926</v>
       </c>
       <c r="B809" t="s">
-        <v>1602</v>
-      </c>
-    </row>
-    <row r="810" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="810" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A810" s="3" t="s">
-        <v>1603</v>
+        <v>1927</v>
       </c>
       <c r="B810" t="s">
-        <v>1604</v>
-      </c>
-    </row>
-    <row r="811" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="811" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A811" s="3" t="s">
-        <v>1605</v>
+        <v>1928</v>
       </c>
       <c r="B811" t="s">
-        <v>1605</v>
-      </c>
-    </row>
-    <row r="812" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="812" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A812" s="3" t="s">
-        <v>1606</v>
+        <v>1929</v>
       </c>
       <c r="B812" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="813" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="813" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A813" s="3" t="s">
-        <v>1607</v>
+        <v>1930</v>
       </c>
       <c r="B813" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="814" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1956</v>
+      </c>
+    </row>
+    <row r="814" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A814" s="3" t="s">
-        <v>1609</v>
+        <v>1931</v>
       </c>
       <c r="B814" t="s">
-        <v>1610</v>
-      </c>
-    </row>
-    <row r="815" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="815" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A815" s="3" t="s">
-        <v>1611</v>
+        <v>1932</v>
       </c>
       <c r="B815" t="s">
-        <v>1612</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="816" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A816" s="3" t="s">
-        <v>1613</v>
+        <v>1933</v>
       </c>
       <c r="B816" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="817" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1959</v>
+      </c>
+    </row>
+    <row r="817" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A817" s="3" t="s">
-        <v>1614</v>
-      </c>
-    </row>
-    <row r="818" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1934</v>
+      </c>
+      <c r="B817" t="s">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="818" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A818" s="3" t="s">
-        <v>1615</v>
-      </c>
-    </row>
-    <row r="819" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1935</v>
+      </c>
+      <c r="B818" t="s">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="819" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A819" s="3" t="s">
-        <v>1616</v>
+        <v>1936</v>
+      </c>
+      <c r="B819" t="s">
+        <v>1962</v>
       </c>
     </row>
     <row r="820" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A820" s="3" t="s">
-        <v>1617</v>
-      </c>
-    </row>
-    <row r="821" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1963</v>
+      </c>
+      <c r="B820" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="821" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A821" s="3" t="s">
-        <v>1618</v>
+        <v>1568</v>
       </c>
       <c r="B821" t="s">
-        <v>1619</v>
-      </c>
-    </row>
-    <row r="822" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="822" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A822" s="3" t="s">
-        <v>1620</v>
+        <v>1569</v>
       </c>
       <c r="B822" t="s">
-        <v>1621</v>
-      </c>
-    </row>
-    <row r="823" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="823" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A823" s="3" t="s">
-        <v>1622</v>
+        <v>1571</v>
       </c>
       <c r="B823" t="s">
-        <v>1623</v>
-      </c>
-    </row>
-    <row r="824" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="824" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A824" s="3" t="s">
-        <v>1624</v>
+        <v>1573</v>
       </c>
       <c r="B824" t="s">
-        <v>1625</v>
-      </c>
-    </row>
-    <row r="825" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="825" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A825" s="3" t="s">
-        <v>1626</v>
+        <v>1575</v>
       </c>
       <c r="B825" t="s">
-        <v>1627</v>
-      </c>
-    </row>
-    <row r="826" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="826" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A826" s="3" t="s">
-        <v>1628</v>
+        <v>1577</v>
       </c>
       <c r="B826" t="s">
-        <v>1629</v>
-      </c>
-    </row>
-    <row r="827" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1578</v>
+      </c>
+    </row>
+    <row r="827" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A827" s="3" t="s">
-        <v>1630</v>
+        <v>1579</v>
       </c>
       <c r="B827" t="s">
-        <v>1631</v>
-      </c>
-    </row>
-    <row r="828" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="828" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A828" s="3" t="s">
-        <v>1632</v>
+        <v>1964</v>
       </c>
       <c r="B828" t="s">
-        <v>1633</v>
-      </c>
-    </row>
-    <row r="829" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="829" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A829" s="3" t="s">
-        <v>1634</v>
+        <v>1966</v>
       </c>
       <c r="B829" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="830" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A830" s="3" t="s">
+        <v>1967</v>
+      </c>
+      <c r="B830" t="s">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="831" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A831" s="3" t="s">
+        <v>1968</v>
+      </c>
+      <c r="B831" t="s">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="832" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A832" s="3" t="s">
+        <v>1969</v>
+      </c>
+      <c r="B832" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="833" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A833" s="3" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B833" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="834" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A834" s="3" t="s">
+        <v>1971</v>
+      </c>
+      <c r="B834" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="835" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A835" s="3" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B835" t="s">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="836" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A836" s="3" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B836" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="837" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A837" s="3" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B837" t="s">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="838" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A838" s="3" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B838" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="839" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A839" s="3" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B839" t="s">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="840" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A840" s="3" t="s">
+        <v>1977</v>
+      </c>
+      <c r="B840" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="841" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A841" s="7" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B841" t="s">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="842" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A842" s="7" t="s">
+        <v>1979</v>
+      </c>
+      <c r="B842" t="s">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="843" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A843" s="7" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B843" t="s">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="844" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A844" s="7" t="s">
+        <v>1981</v>
+      </c>
+      <c r="B844" t="s">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="845" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A845" s="7" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B845" t="s">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="846" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A846" s="7" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B846" t="s">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="847" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A847" s="7" t="s">
+        <v>1984</v>
+      </c>
+      <c r="B847" t="s">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="848" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A848" s="7" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B848" t="s">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="849" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A849" s="7" t="s">
+        <v>1986</v>
+      </c>
+      <c r="B849" t="s">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="850" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A850" s="7" t="s">
+        <v>1987</v>
+      </c>
+      <c r="B850" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="851" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A851" s="7" t="s">
+        <v>1988</v>
+      </c>
+      <c r="B851" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="852" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A852" s="7" t="s">
+        <v>1989</v>
+      </c>
+      <c r="B852" t="s">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="853" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A853" s="7" t="s">
+        <v>1990</v>
+      </c>
+      <c r="B853" t="s">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="854" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A854" s="7" t="s">
+        <v>1991</v>
+      </c>
+      <c r="B854" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="855" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A855" s="7" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B855" t="s">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="856" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A856" s="7" t="s">
+        <v>1993</v>
+      </c>
+      <c r="B856" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="857" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A857" s="7" t="s">
+        <v>1994</v>
+      </c>
+      <c r="B857" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="858" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A858" s="7" t="s">
+        <v>1995</v>
+      </c>
+      <c r="B858" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="859" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A859" s="7" t="s">
+        <v>1996</v>
+      </c>
+      <c r="B859" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="860" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A860" s="7" t="s">
+        <v>1997</v>
+      </c>
+      <c r="B860" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="861" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A861" s="7" t="s">
+        <v>1998</v>
+      </c>
+      <c r="B861" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="862" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A862" s="7" t="s">
+        <v>1999</v>
+      </c>
+      <c r="B862" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="863" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A863" s="7" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B863" t="s">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="864" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A864" s="7" t="s">
+        <v>2001</v>
+      </c>
+      <c r="B864" t="s">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="865" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A865" s="7" t="s">
+        <v>2002</v>
+      </c>
+      <c r="B865" t="s">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="866" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A866" s="7" t="s">
+        <v>2003</v>
+      </c>
+      <c r="B866" t="s">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="867" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A867" s="7" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B867" t="s">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="868" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A868" s="7" t="s">
+        <v>2005</v>
+      </c>
+      <c r="B868" t="s">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="869" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A869" s="7" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B869" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="870" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A870" s="7" t="s">
+        <v>2007</v>
+      </c>
+      <c r="B870" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="871" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A871" s="3" t="s">
+        <v>2050</v>
+      </c>
+      <c r="B871" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="872" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A872" s="3" t="s">
+        <v>2051</v>
+      </c>
+      <c r="B872" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="830" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A830" s="3" t="s">
-        <v>1635</v>
-      </c>
-      <c r="B830" t="s">
-        <v>1636</v>
-      </c>
-    </row>
-    <row r="831" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A831" s="3" t="s">
-        <v>1637</v>
-      </c>
-      <c r="B831" t="s">
-        <v>1638</v>
-      </c>
-    </row>
-    <row r="832" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A832" s="3" t="s">
-        <v>1639</v>
-      </c>
-      <c r="B832" t="s">
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="833" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A833" s="3" t="s">
-        <v>1641</v>
-      </c>
-      <c r="B833" t="s">
-        <v>1642</v>
-      </c>
-    </row>
-    <row r="834" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A834" s="3" t="s">
-        <v>1643</v>
-      </c>
-      <c r="B834" t="s">
-        <v>1644</v>
-      </c>
-    </row>
-    <row r="835" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A835" s="3" t="s">
-        <v>1645</v>
-      </c>
-      <c r="B835" t="s">
-        <v>1646</v>
-      </c>
-    </row>
-    <row r="836" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A836" s="3" t="s">
-        <v>1647</v>
-      </c>
-      <c r="B836" t="s">
-        <v>1648</v>
-      </c>
-    </row>
-    <row r="837" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A837" s="3" t="s">
-        <v>1649</v>
-      </c>
-      <c r="B837" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="838" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A838" s="3" t="s">
-        <v>1650</v>
-      </c>
-      <c r="B838" t="s">
-        <v>1651</v>
-      </c>
-    </row>
-    <row r="839" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A839" s="3" t="s">
-        <v>1652</v>
-      </c>
-      <c r="B839" t="s">
-        <v>1653</v>
-      </c>
-    </row>
-    <row r="840" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A840" s="3" t="s">
-        <v>1654</v>
-      </c>
-      <c r="B840" t="s">
-        <v>1655</v>
-      </c>
-    </row>
-    <row r="841" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A841" s="3" t="s">
-        <v>1656</v>
-      </c>
-      <c r="B841" t="s">
-        <v>1657</v>
-      </c>
-    </row>
-    <row r="842" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A842" s="3" t="s">
-        <v>1658</v>
-      </c>
-      <c r="B842" t="s">
-        <v>1659</v>
-      </c>
-    </row>
-    <row r="843" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A843" s="3" t="s">
-        <v>1660</v>
-      </c>
-      <c r="B843" t="s">
-        <v>1661</v>
-      </c>
-    </row>
-    <row r="844" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A844" s="3" t="s">
-        <v>1662</v>
-      </c>
-      <c r="B844" t="s">
-        <v>1663</v>
-      </c>
-    </row>
-    <row r="845" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A845" s="3" t="s">
-        <v>1664</v>
-      </c>
-      <c r="B845" t="s">
-        <v>1665</v>
-      </c>
-    </row>
-    <row r="846" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A846" s="3" t="s">
-        <v>1666</v>
-      </c>
-      <c r="B846" t="s">
-        <v>1667</v>
-      </c>
-    </row>
-    <row r="847" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A847" s="3" t="s">
-        <v>1668</v>
-      </c>
-      <c r="B847" t="s">
-        <v>1669</v>
-      </c>
-    </row>
-    <row r="848" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A848" s="3" t="s">
-        <v>1670</v>
-      </c>
-      <c r="B848" t="s">
-        <v>1671</v>
-      </c>
-    </row>
-    <row r="849" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A849" s="3" t="s">
-        <v>1672</v>
-      </c>
-      <c r="B849" t="s">
-        <v>1673</v>
-      </c>
-    </row>
-    <row r="850" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A850" s="3" t="s">
-        <v>1674</v>
-      </c>
-      <c r="B850" t="s">
-        <v>1675</v>
-      </c>
-    </row>
-    <row r="851" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A851" s="3" t="s">
-        <v>1676</v>
-      </c>
-      <c r="B851" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="852" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A852" s="3" t="s">
-        <v>1677</v>
-      </c>
-    </row>
-    <row r="853" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A853" s="3" t="s">
-        <v>1678</v>
-      </c>
-      <c r="B853" t="s">
-        <v>1679</v>
-      </c>
-    </row>
-    <row r="854" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A854" s="3" t="s">
-        <v>1680</v>
-      </c>
-      <c r="B854" t="s">
-        <v>1681</v>
-      </c>
-    </row>
-    <row r="855" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A855" s="3" t="s">
-        <v>1682</v>
-      </c>
-      <c r="B855" t="s">
-        <v>1683</v>
-      </c>
-    </row>
-    <row r="856" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A856" s="3" t="s">
-        <v>1684</v>
-      </c>
-      <c r="B856" t="s">
-        <v>1685</v>
-      </c>
-    </row>
-    <row r="857" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A857" s="3" t="s">
-        <v>1686</v>
-      </c>
-      <c r="B857" t="s">
-        <v>1687</v>
-      </c>
-    </row>
-    <row r="858" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A858" s="3" t="s">
-        <v>1688</v>
-      </c>
-      <c r="B858" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="859" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A859" s="3" t="s">
-        <v>1689</v>
-      </c>
-      <c r="B859" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="860" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A860" s="3" t="s">
-        <v>1690</v>
-      </c>
-      <c r="B860" t="s">
-        <v>1691</v>
-      </c>
-    </row>
-    <row r="861" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A861" s="3" t="s">
-        <v>1692</v>
-      </c>
-      <c r="B861" t="s">
-        <v>1693</v>
-      </c>
-    </row>
-    <row r="862" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A862" s="3" t="s">
-        <v>1694</v>
-      </c>
-      <c r="B862" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="863" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A863" s="3" t="s">
-        <v>1696</v>
-      </c>
-      <c r="B863" t="s">
-        <v>1697</v>
-      </c>
-    </row>
-    <row r="864" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A864" s="3" t="s">
-        <v>1698</v>
-      </c>
-      <c r="B864" t="s">
-        <v>1699</v>
-      </c>
-    </row>
-    <row r="865" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A865" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B865" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="866" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A866" s="3" t="s">
-        <v>1701</v>
-      </c>
-      <c r="B866" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="867" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A867" s="3" t="s">
-        <v>1703</v>
-      </c>
-      <c r="B867" t="s">
-        <v>1704</v>
-      </c>
-    </row>
-    <row r="868" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A868" s="3" t="s">
-        <v>1705</v>
-      </c>
-      <c r="B868" t="s">
-        <v>1706</v>
-      </c>
-    </row>
-    <row r="869" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A869" s="3" t="s">
-        <v>1707</v>
-      </c>
-      <c r="B869" t="s">
-        <v>1708</v>
-      </c>
-    </row>
-    <row r="870" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A870" s="3" t="s">
-        <v>1709</v>
-      </c>
-      <c r="B870" t="s">
-        <v>1710</v>
-      </c>
-    </row>
-    <row r="871" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A871" s="3" t="s">
-        <v>1711</v>
-      </c>
-      <c r="B871" t="s">
-        <v>1712</v>
-      </c>
-    </row>
-    <row r="872" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A872" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="B872" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="873" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+    <row r="873" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A873" s="3" t="s">
-        <v>1715</v>
+        <v>2052</v>
       </c>
       <c r="B873" t="s">
-        <v>1716</v>
-      </c>
-    </row>
-    <row r="874" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="874" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A874" s="3" t="s">
-        <v>1717</v>
+        <v>2053</v>
       </c>
       <c r="B874" t="s">
-        <v>12</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="875" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A875" s="3" t="s">
-        <v>1718</v>
+        <v>2054</v>
       </c>
       <c r="B875" t="s">
-        <v>1719</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="876" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A876" s="3" t="s">
-        <v>1720</v>
+        <v>2058</v>
       </c>
       <c r="B876" t="s">
-        <v>1721</v>
+        <v>12</v>
       </c>
     </row>
     <row r="877" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A877" s="3" t="s">
-        <v>1722</v>
+        <v>1581</v>
       </c>
       <c r="B877" t="s">
-        <v>1723</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="878" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A878" s="3" t="s">
-        <v>1724</v>
+        <v>1582</v>
       </c>
       <c r="B878" t="s">
-        <v>1725</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="879" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A879" s="3" t="s">
-        <v>1726</v>
+        <v>1583</v>
       </c>
       <c r="B879" t="s">
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="880" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A880" s="3" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B880" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="880" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A880" s="3" t="s">
-        <v>1727</v>
-      </c>
-      <c r="B880" t="s">
-        <v>1728</v>
-      </c>
-    </row>
-    <row r="881" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+    <row r="881" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A881" s="3" t="s">
-        <v>1729</v>
+        <v>2062</v>
       </c>
       <c r="B881" t="s">
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="882" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>2063</v>
+      </c>
+    </row>
+    <row r="882" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A882" s="3" t="s">
-        <v>1731</v>
+        <v>2064</v>
       </c>
       <c r="B882" t="s">
-        <v>1732</v>
-      </c>
-    </row>
-    <row r="883" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>2096</v>
+      </c>
+    </row>
+    <row r="883" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A883" s="3" t="s">
-        <v>1733</v>
+        <v>2066</v>
       </c>
       <c r="B883" t="s">
-        <v>1734</v>
-      </c>
-    </row>
-    <row r="884" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="884" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A884" s="3" t="s">
-        <v>1735</v>
+        <v>2065</v>
       </c>
       <c r="B884" t="s">
-        <v>1736</v>
-      </c>
-    </row>
-    <row r="885" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="885" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A885" s="3" t="s">
-        <v>1737</v>
+        <v>2067</v>
       </c>
       <c r="B885" t="s">
-        <v>1738</v>
-      </c>
-    </row>
-    <row r="886" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="886" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A886" s="3" t="s">
-        <v>1739</v>
+        <v>2068</v>
       </c>
       <c r="B886" t="s">
-        <v>1740</v>
-      </c>
-    </row>
-    <row r="887" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="887" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A887" s="3" t="s">
-        <v>1741</v>
+        <v>2069</v>
       </c>
       <c r="B887" t="s">
-        <v>1742</v>
-      </c>
-    </row>
-    <row r="888" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>2101</v>
+      </c>
+    </row>
+    <row r="888" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A888" s="3" t="s">
-        <v>1743</v>
-      </c>
-      <c r="B888" s="12" t="s">
-        <v>1743</v>
-      </c>
-    </row>
-    <row r="889" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>2070</v>
+      </c>
+      <c r="B888" t="s">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="889" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A889" s="3" t="s">
-        <v>1744</v>
+        <v>2071</v>
       </c>
       <c r="B889" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A890" s="7" t="s">
+        <v>2072</v>
+      </c>
+      <c r="B890" t="s">
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="891" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A891" s="7" t="s">
+        <v>2073</v>
+      </c>
+      <c r="B891" t="s">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A892" s="7" t="s">
+        <v>2074</v>
+      </c>
+      <c r="B892" t="s">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A893" s="7" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B893" t="s">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="894" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A894" s="7" t="s">
+        <v>2076</v>
+      </c>
+      <c r="B894" t="s">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A895" s="7" t="s">
+        <v>2077</v>
+      </c>
+      <c r="B895" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="896" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A896" s="7" t="s">
+        <v>2078</v>
+      </c>
+      <c r="B896" t="s">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="897" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A897" s="7" t="s">
+        <v>2079</v>
+      </c>
+      <c r="B897" t="s">
+        <v>2111</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A898" s="7" t="s">
+        <v>2080</v>
+      </c>
+      <c r="B898" t="s">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="899" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A899" s="7" t="s">
+        <v>2081</v>
+      </c>
+      <c r="B899" t="s">
+        <v>2113</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A900" s="7" t="s">
+        <v>2082</v>
+      </c>
+      <c r="B900" t="s">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="901" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A901" s="7" t="s">
+        <v>2083</v>
+      </c>
+      <c r="B901" t="s">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="902" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A902" s="7" t="s">
+        <v>2084</v>
+      </c>
+      <c r="B902" t="s">
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="903" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A903" s="7" t="s">
+        <v>2085</v>
+      </c>
+      <c r="B903" t="s">
+        <v>2117</v>
+      </c>
+    </row>
+    <row r="904" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A904" s="7" t="s">
+        <v>2086</v>
+      </c>
+      <c r="B904" t="s">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="905" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A905" s="7" t="s">
+        <v>2087</v>
+      </c>
+      <c r="B905" t="s">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="906" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A906" s="7" t="s">
+        <v>2088</v>
+      </c>
+      <c r="B906" t="s">
+        <v>2119</v>
+      </c>
+    </row>
+    <row r="907" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A907" s="7" t="s">
+        <v>2089</v>
+      </c>
+      <c r="B907" t="s">
+        <v>2121</v>
+      </c>
+    </row>
+    <row r="908" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A908" s="7" t="s">
+        <v>2090</v>
+      </c>
+      <c r="B908" t="s">
+        <v>2122</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A909" s="7" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B909" t="s">
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="910" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A910" s="7" t="s">
+        <v>2092</v>
+      </c>
+      <c r="B910" t="s">
+        <v>2124</v>
+      </c>
+    </row>
+    <row r="911" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A911" s="7" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B911" t="s">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="912" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A912" s="7" t="s">
+        <v>2094</v>
+      </c>
+      <c r="B912" t="s">
+        <v>2126</v>
+      </c>
+    </row>
+    <row r="913" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A913" s="7" t="s">
+        <v>2095</v>
+      </c>
+      <c r="B913" t="s">
+        <v>2127</v>
+      </c>
+    </row>
+    <row r="914" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A914" s="3" t="s">
+        <v>2128</v>
+      </c>
+      <c r="B914" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="890" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A890" s="3" t="s">
-        <v>1745</v>
-      </c>
-      <c r="B890" t="s">
-        <v>1746</v>
-      </c>
-    </row>
-    <row r="891" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A891" s="3" t="s">
-        <v>1747</v>
-      </c>
-      <c r="B891" t="s">
-        <v>1748</v>
-      </c>
-    </row>
-    <row r="892" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A892" s="3" t="s">
-        <v>1749</v>
-      </c>
-      <c r="B892" t="s">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="893" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A893" s="3" t="s">
-        <v>1751</v>
-      </c>
-      <c r="B893" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="894" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A894" s="3" t="s">
-        <v>1752</v>
-      </c>
-      <c r="B894" t="s">
-        <v>1753</v>
-      </c>
-    </row>
-    <row r="895" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A895" s="3" t="s">
-        <v>1754</v>
-      </c>
-      <c r="B895" t="s">
-        <v>1755</v>
-      </c>
-    </row>
-    <row r="896" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A896" s="3" t="s">
-        <v>1756</v>
-      </c>
-      <c r="B896" t="s">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="897" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A897" s="3" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B897" t="s">
-        <v>1759</v>
-      </c>
-    </row>
-    <row r="898" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A898" s="3" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B898" t="s">
-        <v>1761</v>
-      </c>
-    </row>
-    <row r="899" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A899" s="3" t="s">
-        <v>1762</v>
-      </c>
-      <c r="B899" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="900" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A900" s="3" t="s">
-        <v>1763</v>
-      </c>
-      <c r="B900" t="s">
-        <v>1764</v>
-      </c>
-    </row>
-    <row r="901" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A901" s="3" t="s">
-        <v>1765</v>
-      </c>
-      <c r="B901" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="902" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A902" s="3" t="s">
-        <v>1767</v>
-      </c>
-      <c r="B902" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="903" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A903" s="3" t="s">
-        <v>1769</v>
-      </c>
-      <c r="B903" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="904" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A904" s="3" t="s">
-        <v>1771</v>
-      </c>
-      <c r="B904" t="s">
-        <v>1772</v>
-      </c>
-    </row>
-    <row r="905" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A905" s="3" t="s">
-        <v>1773</v>
-      </c>
-      <c r="B905" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="906" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A906" s="3" t="s">
-        <v>1775</v>
-      </c>
-      <c r="B906" t="s">
-        <v>1776</v>
-      </c>
-    </row>
-    <row r="907" spans="1:2" ht="119" x14ac:dyDescent="0.2">
-      <c r="A907" s="3" t="s">
-        <v>1777</v>
-      </c>
-      <c r="B907" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="908" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A908" s="3" t="s">
-        <v>1779</v>
-      </c>
-      <c r="B908" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="909" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A909" s="3" t="s">
-        <v>1780</v>
-      </c>
-      <c r="B909" t="s">
-        <v>1781</v>
-      </c>
-    </row>
-    <row r="910" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A910" s="3" t="s">
-        <v>1782</v>
-      </c>
-      <c r="B910" t="s">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="911" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A911" s="3" t="s">
-        <v>1784</v>
-      </c>
-      <c r="B911" t="s">
-        <v>1785</v>
-      </c>
-    </row>
-    <row r="912" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A912" s="3" t="s">
-        <v>1786</v>
-      </c>
-      <c r="B912" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="913" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A913" s="3" t="s">
-        <v>1788</v>
-      </c>
-      <c r="B913" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="914" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A914" s="3" t="s">
-        <v>1789</v>
-      </c>
-      <c r="B914" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="915" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="915" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A915" s="3" t="s">
-        <v>1791</v>
+        <v>1585</v>
       </c>
       <c r="B915" t="s">
-        <v>1792</v>
-      </c>
-    </row>
-    <row r="916" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="916" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A916" s="3" t="s">
-        <v>1793</v>
+        <v>1587</v>
       </c>
       <c r="B916" t="s">
-        <v>1794</v>
-      </c>
-    </row>
-    <row r="917" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="917" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A917" s="3" t="s">
-        <v>1795</v>
+        <v>1589</v>
       </c>
       <c r="B917" t="s">
-        <v>1796</v>
-      </c>
-    </row>
-    <row r="918" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="918" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A918" s="3" t="s">
-        <v>1797</v>
+        <v>1591</v>
       </c>
       <c r="B918" t="s">
-        <v>1798</v>
-      </c>
-    </row>
-    <row r="919" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="919" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A919" s="3" t="s">
-        <v>1799</v>
+        <v>1593</v>
       </c>
       <c r="B919" t="s">
-        <v>1800</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="920" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A920" s="3" t="s">
-        <v>1801</v>
+        <v>1595</v>
       </c>
       <c r="B920" t="s">
-        <v>12</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="921" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A921" s="3" t="s">
-        <v>1802</v>
+        <v>1597</v>
       </c>
       <c r="B921" t="s">
-        <v>1803</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="922" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A922" s="3" t="s">
-        <v>1804</v>
+        <v>1599</v>
       </c>
       <c r="B922" t="s">
-        <v>1805</v>
+        <v>373</v>
       </c>
     </row>
     <row r="923" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A923" s="3" t="s">
-        <v>1806</v>
+        <v>2129</v>
       </c>
       <c r="B923" t="s">
-        <v>1807</v>
-      </c>
-    </row>
-    <row r="924" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="924" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A924" s="3" t="s">
-        <v>1808</v>
+        <v>2130</v>
       </c>
       <c r="B924" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="925" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>2132</v>
+      </c>
+    </row>
+    <row r="925" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A925" s="3" t="s">
-        <v>1809</v>
+        <v>1600</v>
       </c>
       <c r="B925" t="s">
-        <v>1810</v>
-      </c>
-    </row>
-    <row r="926" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A926" s="3" t="s">
-        <v>1811</v>
-      </c>
-      <c r="B926" t="s">
-        <v>1812</v>
-      </c>
-    </row>
-    <row r="927" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="926" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A926" s="3"/>
+    </row>
+    <row r="927" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A927" s="3" t="s">
-        <v>1813</v>
+        <v>1602</v>
       </c>
       <c r="B927" t="s">
-        <v>1814</v>
-      </c>
-    </row>
-    <row r="928" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="928" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A928" s="3" t="s">
-        <v>1815</v>
+        <v>1604</v>
       </c>
       <c r="B928" t="s">
-        <v>1816</v>
-      </c>
-    </row>
-    <row r="929" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="929" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A929" s="3" t="s">
-        <v>1817</v>
+        <v>1606</v>
       </c>
       <c r="B929" t="s">
-        <v>1818</v>
-      </c>
-    </row>
-    <row r="930" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="930" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A930" s="3" t="s">
-        <v>1819</v>
+        <v>1608</v>
       </c>
       <c r="B930" t="s">
-        <v>1820</v>
-      </c>
-    </row>
-    <row r="931" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="931" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A931" s="3" t="s">
-        <v>1821</v>
+        <v>1610</v>
       </c>
       <c r="B931" t="s">
-        <v>1822</v>
-      </c>
-    </row>
-    <row r="932" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="932" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A932" s="3" t="s">
-        <v>1823</v>
+        <v>1612</v>
       </c>
       <c r="B932" t="s">
-        <v>1824</v>
-      </c>
-    </row>
-    <row r="933" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1613</v>
+      </c>
+    </row>
+    <row r="933" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A933" s="3" t="s">
-        <v>1825</v>
+        <v>1614</v>
       </c>
       <c r="B933" t="s">
-        <v>1826</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="934" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A934" s="3" t="s">
-        <v>1827</v>
+        <v>1616</v>
       </c>
       <c r="B934" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="935" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A935" s="3" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B935" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="936" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A936" s="3" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B936" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="937" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A937" s="3" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B937" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="938" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A938" s="3" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B938" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="939" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A939" s="3" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B939" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="935" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A935" s="3" t="s">
-        <v>1828</v>
-      </c>
-      <c r="B935" t="s">
-        <v>1829</v>
-      </c>
-    </row>
-    <row r="936" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A936" s="3" t="s">
-        <v>1830</v>
-      </c>
-      <c r="B936" t="s">
-        <v>1831</v>
-      </c>
-    </row>
-    <row r="937" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A937" s="3" t="s">
-        <v>1832</v>
-      </c>
-      <c r="B937" t="s">
-        <v>1833</v>
-      </c>
-    </row>
-    <row r="938" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A938" s="3" t="s">
-        <v>1834</v>
-      </c>
-      <c r="B938" t="s">
-        <v>1835</v>
-      </c>
-    </row>
-    <row r="939" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A939" s="3" t="s">
-        <v>1836</v>
-      </c>
-      <c r="B939" t="s">
-        <v>1837</v>
-      </c>
-    </row>
-    <row r="940" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+    <row r="940" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A940" s="3" t="s">
-        <v>1838</v>
-      </c>
-      <c r="B940" t="s">
-        <v>1839</v>
-      </c>
-    </row>
-    <row r="941" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="941" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A941" s="3" t="s">
-        <v>1840</v>
+        <v>1628</v>
       </c>
       <c r="B941" t="s">
-        <v>1841</v>
-      </c>
-    </row>
-    <row r="942" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="942" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A942" s="3" t="s">
-        <v>1842</v>
+        <v>1630</v>
       </c>
       <c r="B942" t="s">
-        <v>1843</v>
-      </c>
-    </row>
-    <row r="943" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="943" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A943" s="3" t="s">
-        <v>1844</v>
+        <v>1632</v>
       </c>
       <c r="B943" t="s">
-        <v>1844</v>
-      </c>
-    </row>
-    <row r="944" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="944" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A944" s="3" t="s">
-        <v>1845</v>
+        <v>1634</v>
       </c>
       <c r="B944" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="945" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="945" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A945" s="3" t="s">
-        <v>1846</v>
+        <v>1636</v>
       </c>
       <c r="B945" t="s">
-        <v>12</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="946" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A946" s="3" t="s">
-        <v>1847</v>
+        <v>1638</v>
       </c>
       <c r="B946" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="947" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="947" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A947" s="3" t="s">
-        <v>1848</v>
+        <v>1639</v>
       </c>
       <c r="B947" t="s">
-        <v>1849</v>
+        <v>12</v>
       </c>
     </row>
     <row r="948" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A948" s="3" t="s">
-        <v>1850</v>
+        <v>1640</v>
       </c>
       <c r="B948" t="s">
-        <v>1851</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="949" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A949" s="3" t="s">
-        <v>1852</v>
+        <v>1642</v>
       </c>
       <c r="B949" t="s">
-        <v>1853</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="950" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A950" s="3" t="s">
-        <v>1854</v>
+        <v>1644</v>
       </c>
       <c r="B950" t="s">
-        <v>1855</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="951" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A951" s="3" t="s">
-        <v>1856</v>
+        <v>1646</v>
       </c>
       <c r="B951" t="s">
-        <v>1857</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="952" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A952" s="3" t="s">
-        <v>1858</v>
+        <v>1648</v>
       </c>
       <c r="B952" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="953" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A953" s="3" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B953" t="s">
         <v>373</v>
-      </c>
-    </row>
-    <row r="953" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A953" s="3" t="s">
-        <v>1859</v>
-      </c>
-      <c r="B953" t="s">
-        <v>1860</v>
       </c>
     </row>
     <row r="954" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A954" s="3" t="s">
-        <v>1861</v>
+        <v>1651</v>
       </c>
       <c r="B954" t="s">
-        <v>1862</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="955" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A955" s="3" t="s">
-        <v>1863</v>
+        <v>1653</v>
       </c>
       <c r="B955" t="s">
-        <v>1864</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="956" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A956" s="3" t="s">
-        <v>1865</v>
+        <v>1655</v>
       </c>
       <c r="B956" t="s">
-        <v>1866</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="957" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A957" s="3" t="s">
-        <v>1867</v>
+        <v>1657</v>
       </c>
       <c r="B957" t="s">
-        <v>1868</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="958" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A958" s="3" t="s">
-        <v>1869</v>
+        <v>1659</v>
       </c>
       <c r="B958" t="s">
-        <v>1870</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="959" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A959" s="3" t="s">
-        <v>1871</v>
+        <v>1661</v>
       </c>
       <c r="B959" t="s">
-        <v>1872</v>
-      </c>
-    </row>
-    <row r="960" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="960" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A960" s="3" t="s">
-        <v>1873</v>
+        <v>1663</v>
       </c>
       <c r="B960" t="s">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="961" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A961" s="3" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B961" t="s">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="962" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A962" s="3" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B962" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="961" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A961" s="3" t="s">
-        <v>1874</v>
-      </c>
-      <c r="B961" t="s">
-        <v>1875</v>
-      </c>
-    </row>
-    <row r="962" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A962" s="3" t="s">
-        <v>1876</v>
-      </c>
-      <c r="B962" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="963" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="963" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A963" s="3" t="s">
-        <v>1878</v>
+        <v>1668</v>
       </c>
       <c r="B963" t="s">
-        <v>1879</v>
-      </c>
-    </row>
-    <row r="964" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="964" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A964" s="3" t="s">
-        <v>1880</v>
+        <v>1670</v>
       </c>
       <c r="B964" t="s">
-        <v>1881</v>
-      </c>
-    </row>
-    <row r="965" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="965" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A965" s="3" t="s">
-        <v>1882</v>
+        <v>1672</v>
       </c>
       <c r="B965" t="s">
-        <v>1883</v>
-      </c>
-    </row>
-    <row r="966" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="966" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A966" s="3" t="s">
-        <v>1884</v>
+        <v>1674</v>
       </c>
       <c r="B966" t="s">
-        <v>1885</v>
-      </c>
-    </row>
-    <row r="967" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="967" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A967" s="3" t="s">
-        <v>1886</v>
+        <v>1676</v>
       </c>
       <c r="B967" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="968" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A968" s="3" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B968" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="969" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A969" s="3" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B969" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="970" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A970" s="3" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B970" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="971" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A971" s="3" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B971" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="972" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A972" s="3" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B972" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="973" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A973" s="3" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B973" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="974" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A974" s="3" t="s">
+        <v>1689</v>
+      </c>
+      <c r="B974" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="975" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A975" s="3" t="s">
+        <v>1691</v>
+      </c>
+      <c r="B975" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="976" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A976" s="3" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B976" s="12" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="977" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A977" s="3" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B977" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="968" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A968" s="3" t="s">
-        <v>1887</v>
-      </c>
-      <c r="B968" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="969" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A969" s="3" t="s">
-        <v>1889</v>
-      </c>
-      <c r="B969" t="s">
-        <v>1890</v>
-      </c>
-    </row>
-    <row r="970" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A970" s="3" t="s">
-        <v>1891</v>
-      </c>
-      <c r="B970" t="s">
-        <v>1892</v>
-      </c>
-    </row>
-    <row r="971" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A971" s="3" t="s">
-        <v>1893</v>
-      </c>
-      <c r="B971" t="s">
-        <v>1894</v>
-      </c>
-    </row>
-    <row r="972" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A972" s="3" t="s">
-        <v>1895</v>
-      </c>
-      <c r="B972" t="s">
-        <v>1896</v>
-      </c>
-    </row>
-    <row r="973" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A973" s="3" t="s">
-        <v>1897</v>
-      </c>
-      <c r="B973" t="s">
-        <v>1898</v>
-      </c>
-    </row>
-    <row r="974" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A974" s="3" t="s">
-        <v>1899</v>
-      </c>
-      <c r="B974" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="975" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A975" s="3" t="s">
-        <v>1900</v>
-      </c>
-      <c r="B975" t="s">
-        <v>1901</v>
-      </c>
-    </row>
-    <row r="976" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A976" s="3" t="s">
-        <v>1902</v>
-      </c>
-      <c r="B976" t="s">
-        <v>1903</v>
-      </c>
-    </row>
-    <row r="977" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A977" s="3" t="s">
-        <v>1904</v>
-      </c>
-      <c r="B977" t="s">
-        <v>1905</v>
       </c>
     </row>
     <row r="978" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A978" s="3" t="s">
-        <v>1906</v>
+        <v>1695</v>
       </c>
       <c r="B978" t="s">
-        <v>1907</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="979" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A979" s="3" t="s">
-        <v>1908</v>
+        <v>1697</v>
       </c>
       <c r="B979" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="980" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="980" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A980" s="3" t="s">
-        <v>1909</v>
+        <v>1699</v>
       </c>
       <c r="B980" t="s">
-        <v>1910</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="981" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A981" s="3" t="s">
-        <v>1911</v>
+        <v>1701</v>
       </c>
       <c r="B981" t="s">
-        <v>1912</v>
-      </c>
-    </row>
-    <row r="982" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="982" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A982" s="3" t="s">
-        <v>1913</v>
+        <v>1702</v>
       </c>
       <c r="B982" t="s">
-        <v>1914</v>
-      </c>
-    </row>
-    <row r="983" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="983" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A983" s="3" t="s">
-        <v>1915</v>
+        <v>1704</v>
       </c>
       <c r="B983" t="s">
-        <v>1916</v>
-      </c>
-    </row>
-    <row r="984" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="984" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A984" s="3" t="s">
-        <v>1917</v>
+        <v>1706</v>
       </c>
       <c r="B984" t="s">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="985" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>1707</v>
+      </c>
+    </row>
+    <row r="985" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A985" s="3" t="s">
-        <v>1919</v>
+        <v>1708</v>
       </c>
       <c r="B985" t="s">
-        <v>1920</v>
-      </c>
-    </row>
-    <row r="986" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="986" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A986" s="3" t="s">
-        <v>1921</v>
+        <v>1710</v>
       </c>
       <c r="B986" t="s">
-        <v>1922</v>
-      </c>
-    </row>
-    <row r="987" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A987" s="1" t="s">
-        <v>1923</v>
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="987" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A987" s="3" t="s">
+        <v>1712</v>
       </c>
       <c r="B987" t="s">
-        <v>1924</v>
-      </c>
-    </row>
-    <row r="988" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="988" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A988" s="3" t="s">
-        <v>1925</v>
+        <v>1713</v>
       </c>
       <c r="B988" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="989" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A989" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B989" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="990" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A990" s="3" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B990" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="991" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A991" s="3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B991" t="s">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="992" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A992" s="3" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B992" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="993" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A993" s="3" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B993" t="s">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="994" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A994" s="3" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B994" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="995" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A995" s="3" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B995" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="996" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A996" s="3" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B996" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="997" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A997" s="3" t="s">
+        <v>1730</v>
+      </c>
+      <c r="B997" t="s">
+        <v>1731</v>
+      </c>
+    </row>
+    <row r="998" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A998" s="3" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B998" t="s">
+        <v>1733</v>
+      </c>
+    </row>
+    <row r="999" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A999" s="3" t="s">
+        <v>1734</v>
+      </c>
+      <c r="B999" t="s">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1000" s="3" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1001" s="3" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B1001" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="989" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A989" s="3" t="s">
-        <v>1926</v>
-      </c>
-      <c r="B989" t="s">
-        <v>1927</v>
-      </c>
-    </row>
-    <row r="990" spans="1:2" ht="170" x14ac:dyDescent="0.2">
-      <c r="A990" s="3" t="s">
-        <v>1928</v>
-      </c>
-      <c r="B990" s="12" t="s">
-        <v>1928</v>
+    <row r="1002" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1002" s="3" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1003" s="3" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1004" s="3" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1005" s="3" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1006" s="3" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1007" s="3" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1008" s="3" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1009" s="3" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1010" s="3" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>1755</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1011" s="3" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1012" s="3" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1013" s="3" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>1760</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1014" s="3" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1015" s="3" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1016" s="3" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1017" s="3" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>1768</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1018" s="3" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1019" s="3" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>1772</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1020" s="3" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1021" s="3" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1022" s="3" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A1023" s="3" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1024" s="3" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1025" s="3" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1026" s="3" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1027" s="3" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1028" s="3" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1029" s="3" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1030" s="3" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1031" s="3" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1032" s="3" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1033" s="3" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1034" s="3" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1035" s="3" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1036" s="3" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B1036" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1037" s="3" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B1037" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1038" s="3" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1039" s="3" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1040" s="3" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1041" s="3" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B1041" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1042" s="3" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1043" s="3" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1044" s="3" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B1044" t="s">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1045" s="3" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1046" s="3" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A1047" s="3" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1048" s="3" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1049" s="3" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1050" s="3" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1051" s="3" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1052" s="3" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1053" s="3" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1054" s="3" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1055" s="3" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1056" s="3" t="s">
+        <v>1837</v>
+      </c>
+      <c r="B1056" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1057" s="3" t="s">
+        <v>1839</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1058" s="3" t="s">
+        <v>1841</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1059" s="3" t="s">
+        <v>1843</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1060" s="3" t="s">
+        <v>1845</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1061" s="3" t="s">
+        <v>1847</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1062" s="3" t="s">
+        <v>1849</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1063" s="3" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1064" s="3" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1065" s="3" t="s">
+        <v>1854</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1066" s="3" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1067" s="3" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1068" s="3" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B1068" t="s">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1069" s="3" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1070" s="3" t="s">
+        <v>1863</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1071" s="3" t="s">
+        <v>1865</v>
+      </c>
+      <c r="B1071" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1072" s="3" t="s">
+        <v>1867</v>
+      </c>
+      <c r="B1072" t="s">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A1073" s="3" t="s">
+        <v>1869</v>
+      </c>
+      <c r="B1073" t="s">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1074" s="3" t="s">
+        <v>1871</v>
+      </c>
+      <c r="B1074" t="s">
+        <v>1872</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1075" s="1" t="s">
+        <v>1873</v>
+      </c>
+      <c r="B1075" t="s">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1076" s="3" t="s">
+        <v>1875</v>
+      </c>
+      <c r="B1076" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1077" s="3" t="s">
+        <v>1876</v>
+      </c>
+      <c r="B1077" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:2" ht="170" x14ac:dyDescent="0.2">
+      <c r="A1078" s="3" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B1078" s="12" t="s">
+        <v>1878</v>
       </c>
     </row>
   </sheetData>
@@ -15396,6 +16642,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010084299BAE6AB37648AD80DEB59DC34125" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3eadf2c1f25cd7b71915c87a24a5e490">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="70b45aa3-433c-4bb7-a757-4861a21b7bcd" xmlns:ns3="f9acbf48-ccda-47b6-abb6-c9eb96c9ba33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="383f12c7747b491aea3350ad3b69b32a" ns2:_="" ns3:_="">
     <xsd:import namespace="70b45aa3-433c-4bb7-a757-4861a21b7bcd"/>
@@ -15566,15 +16821,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B75DB3A7-FCD6-4DD2-8F1A-F1A891316494}">
   <ds:schemaRefs>
@@ -15593,6 +16839,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8739BBC0-A319-48B2-92BB-329AC3208E3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15611,14 +16865,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{14b77578-9773-42d5-8507-251ca2dc2b06}" enabled="0" method="" siteId="{14b77578-9773-42d5-8507-251ca2dc2b06}" removed="1"/>

</xml_diff>

<commit_message>
CHARMS - RAS Updates
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/RASScenario4.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/RASScenario4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bucurgb/IdeaProjects/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F63545-CC9E-F445-9814-324AA150936A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A043CC9-EFA9-7B48-BAF1-D5FC8EEA1999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="58820" yWindow="180" windowWidth="40760" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8595,10 +8595,10 @@
     <t>ScreenerFourProbandLast</t>
   </si>
   <si>
-    <t>SurveyrFourProbandFirst</t>
-  </si>
-  <si>
-    <t>SurveyFourProbandLast</t>
+    <t>SurveyrFourProFirst</t>
+  </si>
+  <si>
+    <t>SurveyFourProLast</t>
   </si>
 </sst>
 </file>
@@ -10017,7 +10017,7 @@
   <dimension ref="A1:B1416"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21510,18 +21510,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21544,14 +21544,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B75DB3A7-FCD6-4DD2-8F1A-F1A891316494}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -21568,6 +21560,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A376A26F-A459-4EA6-9FC7-DF620BE07CA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{14b77578-9773-42d5-8507-251ca2dc2b06}" enabled="0" method="" siteId="{14b77578-9773-42d5-8507-251ca2dc2b06}" removed="1"/>

</xml_diff>